<commit_message>
Updates to finalize model
</commit_message>
<xml_diff>
--- a/team_solutions/Espada/results/Results.xlsx
+++ b/team_solutions/Espada/results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlackHat\Desktop\2023_Quantinuum\team_solutions\Espada\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964657B0-6F9F-4A4F-91F3-B153B2459743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A54187C-45AE-494F-B7C8-BD966F07CB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{7DAF2032-8B19-4B15-9565-57928A4A0111}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
   <si>
     <t>Nelder-Mead</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Quantum Basin Hopping</t>
+  </si>
+  <si>
+    <t>Starting Algorithm</t>
   </si>
 </sst>
 </file>
@@ -115,11 +118,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -129,13 +129,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -452,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE43B09-8ADF-4714-B3C0-BF81D970A765}">
-  <dimension ref="B2:H26"/>
+  <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,17 +462,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -562,21 +559,21 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1">
         <v>88</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="1">
         <v>97</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="1">
         <v>85</v>
       </c>
     </row>
@@ -598,22 +595,22 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>0.46</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="4">
         <v>0.42</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="4">
         <v>0.47</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -700,21 +697,21 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="7">
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1">
         <v>244</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="1">
         <v>260</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="1">
         <v>244</v>
       </c>
     </row>
@@ -736,20 +733,141 @@
       <c r="B26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="4">
         <v>0.42</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <v>0.35</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="4">
         <v>0.27</v>
       </c>
     </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D31" s="1">
+        <v>5000</v>
+      </c>
+      <c r="E31" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1">
+        <v>100</v>
+      </c>
+      <c r="D32" s="1">
+        <v>100</v>
+      </c>
+      <c r="E32" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1">
+        <v>12345</v>
+      </c>
+      <c r="D33" s="1">
+        <v>12345</v>
+      </c>
+      <c r="E33" s="1">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1">
+        <v>7</v>
+      </c>
+      <c r="D34" s="1">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="1">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1">
+        <v>6</v>
+      </c>
+      <c r="E35" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4.9400000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.42</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>